<commit_message>
Adds data to 1-04
</commit_message>
<xml_diff>
--- a/dati_tableau.xlsx
+++ b/dati_tableau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianuccheddu/Desktop/progetti/coronavirus_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0721790C-6379-0E4E-89F3-0424B46B6796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE02CEBB-7571-634E-A662-F8262F0AFCD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{5B5314DD-580D-974E-9D3D-AA62F4E05A27}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dati_1" localSheetId="0">Foglio1!$A$1:$U$667</definedName>
+    <definedName name="dati" localSheetId="0">Foglio1!$A$1:$U$667</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{D8F65504-6131-B74E-8E29-6F5AE01CE0AE}" name="dati" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{150D18AB-0E9A-1042-8BB4-79948D4E6EE2}" name="dati" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/christianuccheddu/Desktop/progetti/coronavirus_analysis/dati.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="21">
         <textField/>
@@ -389,7 +389,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="dati_1" connectionId="1" xr16:uid="{C9165590-BCE7-F946-8FEE-6128AB303C56}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="dati" connectionId="1" xr16:uid="{C2580912-D99D-0A4F-8484-8AF95EB8D8F9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,7 +692,7 @@
   <dimension ref="A1:U685"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>